<commit_message>
Grand avancement du code
Parsing config, et avancement général
</commit_message>
<xml_diff>
--- a/doc/journal/Journal.xlsx
+++ b/doc/journal/Journal.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
   <si>
     <t>DATE</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Rédaction du rapport, partie code, avancement général du code.</t>
+  </si>
+  <si>
+    <t>Avancement du code, fichier config, carte SD application, décodage NMEA, parsing fichier config.</t>
   </si>
 </sst>
 </file>
@@ -557,8 +560,8 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.85546875" defaultRowHeight="45.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -609,7 +612,7 @@
       </c>
       <c r="F2" s="16">
         <f>SUM(E2:E37)</f>
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -833,9 +836,15 @@
       <c r="B17" s="5">
         <v>45160</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="15"/>
+      <c r="C17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">

</xml_diff>

<commit_message>
Avancement du code + journal
</commit_message>
<xml_diff>
--- a/doc/journal/Journal.xlsx
+++ b/doc/journal/Journal.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
   <si>
     <t>DATE</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>Rapport et montage de la carte.</t>
+  </si>
+  <si>
+    <t>Programmation du firmware, lecture/ecriture carte SD, gestion du fichier de config.</t>
+  </si>
+  <si>
+    <t>Programmation du firmware, gestion carte SD, centrale inertielle et GNSS.</t>
   </si>
 </sst>
 </file>
@@ -590,8 +596,8 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.85546875" defaultRowHeight="45.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -642,7 +648,7 @@
       </c>
       <c r="F2" s="16">
         <f>SUM(E2:E37)</f>
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -956,9 +962,13 @@
       <c r="B23" s="5">
         <v>45166</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="C23" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="D23" s="8"/>
-      <c r="E23" s="15"/>
+      <c r="E23" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -967,9 +977,13 @@
       <c r="B24" s="5">
         <v>45167</v>
       </c>
-      <c r="C24" s="6"/>
+      <c r="C24" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="D24" s="8"/>
-      <c r="E24" s="15"/>
+      <c r="E24" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">

</xml_diff>